<commit_message>
Including instances to the case study
</commit_message>
<xml_diff>
--- a/resultados/summary_firstexperiment.xlsx
+++ b/resultados/summary_firstexperiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0.sharepoint.com/sites/GrupodeTrabajodeJusto/Documentos compartidos/General/Routes_Barriers/resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_496DC0BF4345EECF6915609744245E3FB48F8E04" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4832776-465C-49AA-88EC-5F41AB4CC661}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_496DC10FC4435ECFE35A00D542245E3FB48F89FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E24A75A0-CC5F-41B9-97B1-C2A85717D56C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,19 +467,19 @@
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>9</v>
       </c>
       <c r="H2">
-        <v>0.08</v>
+        <v>0.34</v>
       </c>
       <c r="I2">
-        <v>2863.77</v>
+        <v>3601.84</v>
       </c>
       <c r="J2">
-        <v>12.25</v>
+        <v>10.96</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -496,22 +496,22 @@
         <v>0</v>
       </c>
       <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
       <c r="G3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3">
-        <v>0.41</v>
+        <v>0.08</v>
       </c>
       <c r="I3">
-        <v>2920.53</v>
+        <v>2863.77</v>
       </c>
       <c r="J3">
-        <v>11.77</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -525,24 +525,56 @@
         <v>18</v>
       </c>
       <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>0.41</v>
+      </c>
+      <c r="I4">
+        <v>2920.53</v>
+      </c>
+      <c r="J4">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>9</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>0.46</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>2868.93</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <v>8.48</v>
       </c>
     </row>
@@ -809,13 +841,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C81E281-35A1-477C-A6CC-258A520460AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B532B5-3193-4B14-90C2-3CBB78956810}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D029027-B109-48AA-9ADB-A12E125DD4E9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BDA46B4-C2C6-4860-8087-2A87282C2287}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8563D8-4003-4489-9AB3-65D0A782CADA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA4432C-BAC0-4B98-81C4-5C5EB4DB7787}"/>
 </file>
</xml_diff>

<commit_message>
Cambios en la version de latex y la carta.
</commit_message>
<xml_diff>
--- a/resultados/summary_firstexperiment.xlsx
+++ b/resultados/summary_firstexperiment.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0.sharepoint.com/sites/GrupodeTrabajodeJusto/Documentos compartidos/General/Routes_Barriers/resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_496DC10FC4435ECFE35A00D542245E3FB48F89FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E24A75A0-CC5F-41B9-97B1-C2A85717D56C}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_3A6E09F6E93915C12799AF2DB7E7814B10B37F22" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{337D7C5C-64CA-44B8-B909-EC7B7117A93A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>n_N</t>
   </si>
@@ -47,6 +60,12 @@
   </si>
   <si>
     <t>Time_Prepro</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -75,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -84,17 +103,51 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -102,9 +155,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -122,6 +208,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,176 +499,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3601.4</v>
+      </c>
+      <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2">
-        <v>0.34</v>
-      </c>
-      <c r="I2">
-        <v>3601.84</v>
-      </c>
-      <c r="J2">
-        <v>10.96</v>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2863.76</v>
+      </c>
+      <c r="I3" s="2">
+        <v>6.62</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>18</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3">
-        <v>0.08</v>
-      </c>
-      <c r="I3">
-        <v>2863.77</v>
-      </c>
-      <c r="J3">
-        <v>12.25</v>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2920.99</v>
+      </c>
+      <c r="I4" s="2">
+        <v>5.31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>0.41</v>
-      </c>
-      <c r="I4">
-        <v>2920.53</v>
-      </c>
-      <c r="J4">
-        <v>11.77</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2643.25</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>0.46</v>
-      </c>
-      <c r="I5">
-        <v>2868.93</v>
-      </c>
-      <c r="J5">
-        <v>8.48</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1453.59</v>
+      </c>
+      <c r="I6" s="9">
+        <v>7.55</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -829,25 +926,29 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="116ddbad-b67c-4622-b846-55da43670eb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0838a0db-6cb4-4fef-a3f8-577e3ea6a4fe" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B532B5-3193-4B14-90C2-3CBB78956810}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A722-5653-4A16-8791-602060209C20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="116ddbad-b67c-4622-b846-55da43670eb8"/>
+    <ds:schemaRef ds:uri="0838a0db-6cb4-4fef-a3f8-577e3ea6a4fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BDA46B4-C2C6-4860-8087-2A87282C2287}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA4432C-BAC0-4B98-81C4-5C5EB4DB7787}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75823394-B27F-4DD6-B367-D06B2FC69085}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>